<commit_message>
Images and PCB Update
</commit_message>
<xml_diff>
--- a/pcbs/Transmitter/BOM.xlsx
+++ b/pcbs/Transmitter/BOM.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="BOM_Board1_PCB1_2025-10-23" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="BOM_Board1_PCB1_2025-11-27" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>No.</t>
   </si>
@@ -46,25 +46,85 @@
     <t>1</t>
   </si>
   <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>C1,C2</t>
+  </si>
+  <si>
+    <t>C0402</t>
+  </si>
+  <si>
+    <t>CL05A105KO5NNNC</t>
+  </si>
+  <si>
+    <t>SAMSUNG(三星)</t>
+  </si>
+  <si>
+    <t>C29266</t>
+  </si>
+  <si>
+    <t>LCSC</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>100kΩ</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>RC0402FR-07100KL</t>
+  </si>
+  <si>
+    <t>YAGEO(国巨)</t>
+  </si>
+  <si>
+    <t>C60491</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>ESP32-S3-Zero</t>
   </si>
   <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>COMM-SMD_18P-P2.54-L23.5-W18.0-TL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>C9900152785</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>TPS22918DBVR</t>
+  </si>
+  <si>
     <t>U2</t>
   </si>
   <si>
-    <t>COMM-SMD_18P-P2.54-L23.5-W18.0-TL</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>C9900152785</t>
-  </si>
-  <si>
-    <t>LCSC</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>SOT-23-6_L2.9-W1.6-P0.95-LS2.8-BR</t>
+  </si>
+  <si>
+    <t>TI(德州仪器)</t>
+  </si>
+  <si>
+    <t>C131941</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t>ZX-SH1.0-5PWT</t>
@@ -456,7 +516,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -502,7 +562,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -514,56 +574,152 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>